<commit_message>
adding DaemonSet and Logging
</commit_message>
<xml_diff>
--- a/Version_Details.xlsx
+++ b/Version_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chordia\Documents\Github\kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7287260-5F5A-4BB7-BA31-E16BB53E8158}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E7CBC0-7195-4FAE-ABD1-E6560E5F4B8F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{704E2FE4-463B-4293-93D8-01347A6C7E26}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>kind</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>Binding</t>
+  </si>
+  <si>
+    <t>LimitRange</t>
+  </si>
+  <si>
+    <t>ResourceQuota</t>
+  </si>
+  <si>
+    <t>DaemonSet</t>
   </si>
 </sst>
 </file>
@@ -453,7 +462,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,16 +528,28 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>

</xml_diff>